<commit_message>
changed method of loading in data and metadata
</commit_message>
<xml_diff>
--- a/data/DRUG_CLASS_I_Mean_Cmax_Trough_Efficacy_R_DATA_ANALYSIS.xlsx
+++ b/data/DRUG_CLASS_I_Mean_Cmax_Trough_Efficacy_R_DATA_ANALYSIS.xlsx
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2186,93 +2186,93 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C30" s="1" t="s">
+      <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="10"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="10"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="10"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="10"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="10"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="10"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="10"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="10"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="10"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="10"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>48</v>
       </c>

</xml_diff>